<commit_message>
fixed #2939 Änderungen in Feldbezeichnungen
</commit_message>
<xml_diff>
--- a/conf/conf.xlsx
+++ b/conf/conf.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
   <si>
     <t>ID</t>
   </si>
@@ -299,10 +299,10 @@
     <t xml:space="preserve">Darstellung im Riss (auch Instrumentenstandpunkte)</t>
   </si>
   <si>
-    <t>Zuverlässigkeit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zuverlässigkeit des Lageanschlusses (Anzahl, Verteilung…) gemäß 4.3.2 LiVermVV</t>
+    <t xml:space="preserve">Zulässigkeit des Lageanschlusses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zulässigkeit des Lageanschlusses (Anzahl, Verteilung…) gemäß 4.3.2 LiVermVV</t>
   </si>
   <si>
     <t>Dokumentation</t>
@@ -338,11 +338,14 @@
     <t xml:space="preserve">Angabe der verwendeten Unterlagen (mit Buchstaben) </t>
   </si>
   <si>
-    <t xml:space="preserve">Nachweis Punktidentität</t>
+    <t xml:space="preserve">Nachweis Punktidentität Vermessungsriss</t>
   </si>
   <si>
     <t xml:space="preserve">Nachweis der Punktidentität, siehe 5.1.1 LiVermVV (Gegenüberstellung: Katasterzahlen&lt;&gt;Ergebnis der 
 Grenzermittlung) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nachweis Punktidentität Koordinatenverzeichnis</t>
   </si>
   <si>
     <t xml:space="preserve">Nachweis der Punktidentität im Koordinatenkastaster gemäß 5.1.1 LiVermVV (Sollkoordinate&lt;&gt;Istkoordinate,
@@ -748,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -774,6 +777,7 @@
     </xf>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -782,6 +786,9 @@
     </xf>
     <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1315,7 +1322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1486,7 +1493,7 @@
       <c r="G6" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -2367,10 +2374,10 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="13" t="s">
         <v>94</v>
       </c>
       <c r="D37" t="s">
@@ -2541,10 +2548,10 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="15" t="s">
         <v>107</v>
       </c>
       <c r="D43" t="s">
@@ -2570,11 +2577,11 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C44" s="15" t="s">
+      <c r="B44" s="14" t="s">
         <v>108</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="D44" t="s">
         <v>103</v>
@@ -2600,10 +2607,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D45" t="s">
         <v>103</v>
@@ -2629,10 +2636,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D46" t="s">
         <v>103</v>
@@ -2658,13 +2665,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E47" t="s">
         <v>22</v>
@@ -2687,13 +2694,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" t="s">
         <v>115</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D48" t="s">
-        <v>114</v>
       </c>
       <c r="E48" t="s">
         <v>22</v>
@@ -2716,13 +2723,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D49" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E49" t="s">
         <v>22</v>
@@ -2744,14 +2751,14 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C50" s="14" t="s">
+      <c r="B50" s="17" t="s">
         <v>120</v>
       </c>
+      <c r="C50" s="15" t="s">
+        <v>121</v>
+      </c>
       <c r="D50" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E50" t="s">
         <v>22</v>
@@ -2773,14 +2780,14 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D51" t="s">
         <v>122</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D51" t="s">
-        <v>121</v>
       </c>
       <c r="E51" t="s">
         <v>22</v>
@@ -2803,13 +2810,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D52" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E52" t="s">
         <v>22</v>
@@ -2832,13 +2839,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D53" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E53" t="s">
         <v>22</v>
@@ -2860,14 +2867,14 @@
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C54" s="16" t="s">
+      <c r="B54" s="17" t="s">
         <v>129</v>
       </c>
+      <c r="C54" s="18" t="s">
+        <v>130</v>
+      </c>
       <c r="D54" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E54" t="s">
         <v>22</v>
@@ -2890,13 +2897,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D55" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E55" t="s">
         <v>22</v>
@@ -2919,13 +2926,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D56" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E56" t="s">
         <v>22</v>
@@ -2948,13 +2955,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D57" t="s">
         <v>135</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D57" t="s">
-        <v>134</v>
       </c>
       <c r="E57" t="s">
         <v>22</v>
@@ -2977,13 +2984,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D58" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E58" t="s">
         <v>22</v>
@@ -3005,14 +3012,14 @@
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C59" s="17" t="s">
+      <c r="B59" s="19" t="s">
         <v>138</v>
       </c>
+      <c r="C59" s="19" t="s">
+        <v>139</v>
+      </c>
       <c r="D59" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E59" t="s">
         <v>22</v>
@@ -3034,14 +3041,14 @@
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D60" t="s">
         <v>140</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D60" t="s">
-        <v>139</v>
       </c>
       <c r="E60" t="s">
         <v>22</v>
@@ -3063,14 +3070,14 @@
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="C61" s="18" t="s">
-        <v>142</v>
+      <c r="B61" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>143</v>
       </c>
       <c r="D61" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E61" t="s">
         <v>22</v>
@@ -3092,14 +3099,14 @@
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="D62" t="s">
         <v>144</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D62" t="s">
-        <v>143</v>
       </c>
       <c r="E62" t="s">
         <v>22</v>
@@ -3121,14 +3128,14 @@
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" s="18" t="s">
+      <c r="B63" s="20" t="s">
         <v>147</v>
       </c>
+      <c r="C63" s="20" t="s">
+        <v>148</v>
+      </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E63" t="s">
         <v>22</v>
@@ -3150,14 +3157,14 @@
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="C64" s="19" t="s">
+      <c r="B64" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="C64" s="21" t="s">
         <v>150</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="E64" t="s">
         <v>22</v>
@@ -3179,14 +3186,14 @@
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="C65" s="21" t="s">
+      <c r="B65" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D65" s="21" t="s">
         <v>151</v>
-      </c>
-      <c r="D65" s="19" t="s">
-        <v>150</v>
       </c>
       <c r="E65" t="s">
         <v>22</v>
@@ -3209,10 +3216,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C66" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E66" t="s">
         <v>22</v>
@@ -3224,7 +3231,7 @@
         <v>13</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3247,142 +3254,141 @@
     <col customWidth="1" min="1" max="1" width="37.7109375"/>
     <col customWidth="1" min="2" max="2" width="19"/>
     <col customWidth="1" min="3" max="3" width="19.85546875"/>
-    <col min="4" max="16384" width="11.421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="D1" s="24" t="s">
         <v>159</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="B7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="B8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="B9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="B10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="B11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="B12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="B13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="B14" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="B15" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3406,102 +3412,102 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="24"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="D3" s="24"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="26"/>
     </row>
     <row r="4">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="D5" s="28"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="30"/>
     </row>
     <row r="6">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
     </row>
     <row r="7">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="24"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="26"/>
     </row>
     <row r="8">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
     </row>
     <row r="9">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="24"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="26"/>
     </row>
     <row r="10">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
     </row>
     <row r="11">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="D11" s="24"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="26"/>
     </row>
     <row r="12">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
     </row>
     <row r="13">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="D13" s="24"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="26"/>
     </row>
     <row r="14">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3531,52 +3537,52 @@
   <sheetData>
     <row r="2">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>